<commit_message>
Added number keyboard with live view
</commit_message>
<xml_diff>
--- a/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
+++ b/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10881" uniqueCount="182">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -195,6 +195,428 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle Logical LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Witaj w programie inteligenta butelka!
+Klikni START aby rozpocząć &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wprowadź swoje dane:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zatwierdź</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Witaj w programie inteligenta butelka!
+Klikni START aby rozpocząć &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Witaj w programie inteligenta butelka!
+Klikni START aby rozpocząć &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Witaj w programie inteligenta butelka!
+Klikni START aby rozpocząć &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure you want to reset?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure to reset?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wprowadź dane:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waga:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wzrost:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnoć</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wzrost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STARrrrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pojemnosc
+ butelki</t>
   </si>
 </sst>
 </file>
@@ -1473,9 +1895,7 @@
         <v>17</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
+      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
@@ -1676,7 +2096,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1688,75 +2108,449 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>57</v>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working user data input via number keyboard
</commit_message>
<xml_diff>
--- a/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
+++ b/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10881" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11281" uniqueCount="189">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -617,6 +617,27 @@
   <si>
     <t xml:space="preserve">Pojemnosc
  butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twoje zapotrzebowanie na wodę wynosi:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
   </si>
 </sst>
 </file>
@@ -2431,7 +2452,7 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25">
@@ -2465,7 +2486,7 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27">
@@ -2533,7 +2554,7 @@
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
@@ -2551,6 +2572,74 @@
       </c>
       <c r="F31" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added deleting variables in screen 2
</commit_message>
<xml_diff>
--- a/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
+++ b/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11281" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13407" uniqueCount="200">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -638,6 +638,39 @@
   </si>
   <si>
     <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wynik: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reszta: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x &lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123445</t>
   </si>
 </sst>
 </file>
@@ -2440,7 +2473,7 @@
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -2457,7 +2490,7 @@
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -2474,92 +2507,92 @@
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>125</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
@@ -2571,12 +2604,12 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
@@ -2588,60 +2621,15 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="s">
-        <v>183</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" t="s">
-        <v>188</v>
-      </c>
-    </row>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added pojemnosc and water calculations
</commit_message>
<xml_diff>
--- a/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
+++ b/touch_display/F4_GFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19635" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22151" uniqueCount="258">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -815,6 +815,71 @@
   <si>
     <t xml:space="preserve">Twoje zapotrzebowanie 
 na wodę wynosi:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wysoko
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wysokoć
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wysokosc
+ butelki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy na pewno chcesz zresetowac ustawienia? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy na pewno chcesz 
+zresetowac ustawienia? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy na pewno chcesz 
+zresetowac ustawienia? </t>
   </si>
 </sst>
 </file>
@@ -2544,7 +2609,7 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20">
@@ -2561,7 +2626,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21">
@@ -2578,7 +2643,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22">
@@ -2731,7 +2796,7 @@
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31">
@@ -2782,7 +2847,7 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34">
@@ -2799,7 +2864,7 @@
         <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35">
@@ -2816,7 +2881,7 @@
         <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36">
@@ -2833,7 +2898,7 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37">
@@ -2850,10 +2915,111 @@
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>242</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>244</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>245</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>